<commit_message>
Datos planta y simulink para el brazo, necesitamos hacer simulación del experimento de fuerza vs ángulo y del movimiento subamortiguado
</commit_message>
<xml_diff>
--- a/control_brazo/diagrama_pwm_vs_angulo.xlsx
+++ b/control_brazo/diagrama_pwm_vs_angulo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive\Documents\Universidad\Control\control_brazo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0409421D-792F-490D-B2BB-A1F8E129CF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2067E26E-B13C-4179-820B-A3C63C15FEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{07C319F7-47B6-4E78-9131-C3B5DCC281C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Contrapeso moneda y llave </t>
   </si>
@@ -44,10 +44,13 @@
     <t>Pwm</t>
   </si>
   <si>
-    <t xml:space="preserve">Ángulo </t>
+    <t>Pwm_%</t>
   </si>
   <si>
-    <t>Pwm_%</t>
+    <t>Ángulo (Deg)</t>
+  </si>
+  <si>
+    <t>Ángulo (Rad)</t>
   </si>
 </sst>
 </file>
@@ -158,11 +161,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$1</c:f>
+              <c:f>Hoja1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ángulo </c:v>
+                  <c:v>Ángulo (Rad)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -225,144 +228,144 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$22</c:f>
+              <c:f>Hoja1!$A$2:$A$22</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8875855327468229E-2</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.7751710654936458E-2</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1466275659824047</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19550342130987292</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24437927663734116</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2932551319648094</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.34213098729227759</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39100684261974583</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.43988269794721407</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.48875855327468232</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.5376344086021505</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5865102639296188</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.63538611925708699</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.68426197458455518</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.73313782991202348</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.78201368523949166</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.83088954056695996</c:v>
+                  <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.87976539589442815</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.92864125122189634</c:v>
+                  <c:v>950</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.97751710654936463</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$22</c:f>
+              <c:f>Hoja1!$D$2:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-1.76</c:v>
+                  <c:v>-3.0717794835100197E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7</c:v>
+                  <c:v>1.2217304763960306E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.52</c:v>
+                  <c:v>6.1435589670200394E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.69</c:v>
+                  <c:v>0.11676252695842064</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.15</c:v>
+                  <c:v>0.15969762655748115</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.96</c:v>
+                  <c:v>0.20874137853852182</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.78</c:v>
+                  <c:v>0.2579596634447619</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.89</c:v>
+                  <c:v>0.29478611066184224</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.649999999999999</c:v>
+                  <c:v>0.32550390549694241</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.11</c:v>
+                  <c:v>0.35098571257605965</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23.23</c:v>
+                  <c:v>0.40543998523828279</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.34</c:v>
+                  <c:v>0.44226643245536312</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.1</c:v>
+                  <c:v>0.4729842272904633</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28.5</c:v>
+                  <c:v>0.49741883681838389</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30.62</c:v>
+                  <c:v>0.53441981696066376</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34.130000000000003</c:v>
+                  <c:v>0.59568087370566469</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35.89</c:v>
+                  <c:v>0.62639866854076487</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>37.299999999999997</c:v>
+                  <c:v>0.65100781099388483</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>39.06</c:v>
+                  <c:v>0.68172560582898512</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>40.119999999999997</c:v>
+                  <c:v>0.70022609590012497</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42.23</c:v>
+                  <c:v>0.73705254311720536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -393,7 +396,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1493,7 +1496,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1506,10 +1509,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="D1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1522,6 +1528,10 @@
       <c r="C2">
         <v>-1.76</v>
       </c>
+      <c r="D2">
+        <f>C2*PI()/180</f>
+        <v>-3.0717794835100197E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -1534,17 +1544,25 @@
       <c r="C3">
         <v>0.7</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D22" si="0">C3*PI()/180</f>
+        <v>1.2217304763960306E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>100</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B22" si="0">A4/1023</f>
+        <f t="shared" ref="B4:B22" si="1">A4/1023</f>
         <v>9.7751710654936458E-2</v>
       </c>
       <c r="C4">
         <v>3.52</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>6.1435589670200394E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1552,11 +1570,15 @@
         <v>150</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1466275659824047</v>
       </c>
       <c r="C5">
         <v>6.69</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.11676252695842064</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -1567,11 +1589,15 @@
         <v>200</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19550342130987292</v>
       </c>
       <c r="C6">
         <v>9.15</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.15969762655748115</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1579,11 +1605,15 @@
         <v>250</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.24437927663734116</v>
       </c>
       <c r="C7">
         <v>11.96</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.20874137853852182</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1591,11 +1621,15 @@
         <v>300</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2932551319648094</v>
       </c>
       <c r="C8">
         <v>14.78</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.2579596634447619</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1603,11 +1637,15 @@
         <v>350</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.34213098729227759</v>
       </c>
       <c r="C9">
         <v>16.89</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.29478611066184224</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1615,11 +1653,15 @@
         <v>400</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.39100684261974583</v>
       </c>
       <c r="C10">
         <v>18.649999999999999</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.32550390549694241</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1627,11 +1669,15 @@
         <v>450</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.43988269794721407</v>
       </c>
       <c r="C11">
         <v>20.11</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.35098571257605965</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1639,11 +1685,15 @@
         <v>500</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.48875855327468232</v>
       </c>
       <c r="C12">
         <v>23.23</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.40543998523828279</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1651,11 +1701,15 @@
         <v>550</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5376344086021505</v>
       </c>
       <c r="C13">
         <v>25.34</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.44226643245536312</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1663,11 +1717,15 @@
         <v>600</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5865102639296188</v>
       </c>
       <c r="C14">
         <v>27.1</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.4729842272904633</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1675,11 +1733,15 @@
         <v>650</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.63538611925708699</v>
       </c>
       <c r="C15">
         <v>28.5</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.49741883681838389</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1687,83 +1749,111 @@
         <v>700</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.68426197458455518</v>
       </c>
       <c r="C16">
         <v>30.62</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.53441981696066376</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>750</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.73313782991202348</v>
       </c>
       <c r="C17">
         <v>34.130000000000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.59568087370566469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>800</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.78201368523949166</v>
       </c>
       <c r="C18">
         <v>35.89</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.62639866854076487</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>850</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83088954056695996</v>
       </c>
       <c r="C19">
         <v>37.299999999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0.65100781099388483</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>900</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.87976539589442815</v>
       </c>
       <c r="C20">
         <v>39.06</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0.68172560582898512</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>950</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.92864125122189634</v>
       </c>
       <c r="C21">
         <v>40.119999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.70022609590012497</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1000</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.97751710654936463</v>
       </c>
       <c r="C22">
         <v>42.23</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0.73705254311720536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Control brazo actualizado y clase de variables de estados
</commit_message>
<xml_diff>
--- a/control_brazo/diagrama_pwm_vs_angulo.xlsx
+++ b/control_brazo/diagrama_pwm_vs_angulo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive\Documents\Universidad\Control\control_brazo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2067E26E-B13C-4179-820B-A3C63C15FEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9899702-044E-4BC5-A172-27877C93E95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{07C319F7-47B6-4E78-9131-C3B5DCC281C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t xml:space="preserve">Contrapeso moneda y llave </t>
   </si>
@@ -57,8 +58,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -86,9 +95,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1496,7 +1506,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1544,8 +1554,8 @@
       <c r="C3">
         <v>0.7</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D22" si="0">C3*PI()/180</f>
+      <c r="D3" s="2">
+        <f>C3*PI()/180</f>
         <v>1.2217304763960306E-2</v>
       </c>
     </row>
@@ -1554,14 +1564,14 @@
         <v>100</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B22" si="1">A4/1023</f>
+        <f t="shared" ref="B4:B22" si="0">A4/1023</f>
         <v>9.7751710654936458E-2</v>
       </c>
       <c r="C4">
         <v>3.52</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D3:D22" si="1">C4*PI()/180</f>
         <v>6.1435589670200394E-2</v>
       </c>
     </row>
@@ -1570,14 +1580,14 @@
         <v>150</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1466275659824047</v>
       </c>
       <c r="C5">
         <v>6.69</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11676252695842064</v>
       </c>
       <c r="E5" t="s">
@@ -1589,14 +1599,14 @@
         <v>200</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.19550342130987292</v>
       </c>
       <c r="C6">
         <v>9.15</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15969762655748115</v>
       </c>
     </row>
@@ -1605,14 +1615,14 @@
         <v>250</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.24437927663734116</v>
       </c>
       <c r="C7">
         <v>11.96</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.20874137853852182</v>
       </c>
     </row>
@@ -1621,14 +1631,14 @@
         <v>300</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.2932551319648094</v>
       </c>
       <c r="C8">
         <v>14.78</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2579596634447619</v>
       </c>
     </row>
@@ -1637,14 +1647,14 @@
         <v>350</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.34213098729227759</v>
       </c>
       <c r="C9">
         <v>16.89</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29478611066184224</v>
       </c>
     </row>
@@ -1653,14 +1663,14 @@
         <v>400</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.39100684261974583</v>
       </c>
       <c r="C10">
         <v>18.649999999999999</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.32550390549694241</v>
       </c>
     </row>
@@ -1669,14 +1679,14 @@
         <v>450</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.43988269794721407</v>
       </c>
       <c r="C11">
         <v>20.11</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.35098571257605965</v>
       </c>
     </row>
@@ -1685,14 +1695,14 @@
         <v>500</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.48875855327468232</v>
       </c>
       <c r="C12">
         <v>23.23</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40543998523828279</v>
       </c>
     </row>
@@ -1701,14 +1711,14 @@
         <v>550</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5376344086021505</v>
       </c>
       <c r="C13">
         <v>25.34</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.44226643245536312</v>
       </c>
     </row>
@@ -1717,14 +1727,14 @@
         <v>600</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5865102639296188</v>
       </c>
       <c r="C14">
         <v>27.1</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4729842272904633</v>
       </c>
     </row>
@@ -1733,14 +1743,14 @@
         <v>650</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.63538611925708699</v>
       </c>
       <c r="C15">
         <v>28.5</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.49741883681838389</v>
       </c>
     </row>
@@ -1749,14 +1759,14 @@
         <v>700</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.68426197458455518</v>
       </c>
       <c r="C16">
         <v>30.62</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.53441981696066376</v>
       </c>
     </row>
@@ -1765,14 +1775,14 @@
         <v>750</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.73313782991202348</v>
       </c>
       <c r="C17">
         <v>34.130000000000003</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.59568087370566469</v>
       </c>
     </row>
@@ -1781,14 +1791,14 @@
         <v>800</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.78201368523949166</v>
       </c>
       <c r="C18">
         <v>35.89</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.62639866854076487</v>
       </c>
     </row>
@@ -1797,14 +1807,14 @@
         <v>850</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.83088954056695996</v>
       </c>
       <c r="C19">
         <v>37.299999999999997</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.65100781099388483</v>
       </c>
     </row>
@@ -1813,14 +1823,14 @@
         <v>900</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.87976539589442815</v>
       </c>
       <c r="C20">
         <v>39.06</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.68172560582898512</v>
       </c>
     </row>
@@ -1829,14 +1839,14 @@
         <v>950</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.92864125122189634</v>
       </c>
       <c r="C21">
         <v>40.119999999999997</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.70022609590012497</v>
       </c>
     </row>
@@ -1845,14 +1855,14 @@
         <v>1000</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.97751710654936463</v>
       </c>
       <c r="C22">
         <v>42.23</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.73705254311720536</v>
       </c>
     </row>
@@ -1860,4 +1870,217 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C889F156-EA85-4AFB-AF2A-418757B7A271}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>A2*PI()/180</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B22" si="0">A3*PI()/180</f>
+        <v>0.87266462599716477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>1.7453292519943295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>150</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>2.6179938779914944</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>200</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>3.4906585039886591</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>250</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>4.3633231299858233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>300</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829888</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>350</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>6.1086523819801526</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>400</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>6.9813170079773181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>450</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>7.8539816339744828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>500</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>8.7266462599716466</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>550</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>9.5993108859688121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>600</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>10.471975511965978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>650</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>11.344640137963141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>700</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>12.217304763960305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>750</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>13.089969389957471</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>800</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>13.962634015954636</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>850</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>14.8352986419518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>900</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>15.707963267948966</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>950</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>16.580627893946129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1000</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>17.453292519943293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>